<commit_message>
arrivati a versione 1.0.0
</commit_message>
<xml_diff>
--- a/riassuntoAutomatico.xlsx
+++ b/riassuntoAutomatico.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="311">
   <si>
     <t>Riassunto analisi</t>
   </si>
   <si>
-    <t>Trovati errori per 81 bambini</t>
+    <t>Trovati errori per 82 bambini</t>
   </si>
   <si>
     <t>Trovate 3 occorrenze per il controllo Controllo età bambino</t>
@@ -34,6 +34,9 @@
     <t>Trovate 24 occorrenze per il controllo Controllo Kindergarten #2</t>
   </si>
   <si>
+    <t>Trovate 1 occorrenze per il controllo Contratti lockdown sospetti (Covid #4)</t>
+  </si>
+  <si>
     <t>Trovate 8 occorrenze per il controllo Controllo Fehler Eingewöhnung</t>
   </si>
   <si>
@@ -559,6 +562,18 @@
     <t>2017-11-13 00:00:00</t>
   </si>
   <si>
+    <t>Contratti lockdown sospetti (Covid #4)</t>
+  </si>
+  <si>
+    <t>SANTON PHILIPP</t>
+  </si>
+  <si>
+    <t>SNTPLP19A31B220R</t>
+  </si>
+  <si>
+    <t>2019-01-31 00:00:00</t>
+  </si>
+  <si>
     <t>Controllo Fehler Eingewöhnung</t>
   </si>
   <si>
@@ -835,10 +850,10 @@
     <t>2017-08-13 00:00:00</t>
   </si>
   <si>
+    <t>Plaus</t>
+  </si>
+  <si>
     <t>Laas</t>
-  </si>
-  <si>
-    <t>Plaus</t>
   </si>
   <si>
     <t>KOFLER PAULI</t>
@@ -1272,7 +1287,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E173"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1343,103 +1358,94 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="B20" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
         <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C23" t="s">
         <v>23</v>
       </c>
-      <c r="E22" t="s">
+      <c r="D23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
+      <c r="E23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" t="s">
         <v>27</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C27" t="s">
         <v>28</v>
       </c>
-      <c r="E26" t="s">
+      <c r="D27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1" t="s">
+      <c r="E27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" t="s">
         <v>35</v>
-      </c>
-      <c r="C31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1447,1691 +1453,1724 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
         <v>39</v>
       </c>
-      <c r="C33" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" t="s">
-        <v>41</v>
-      </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
         <v>42</v>
       </c>
-      <c r="C34" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" t="s">
-        <v>44</v>
-      </c>
       <c r="E34" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" t="s">
         <v>46</v>
-      </c>
-      <c r="C35" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
         <v>49</v>
       </c>
-      <c r="C36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" t="s">
-        <v>51</v>
-      </c>
       <c r="E36" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
         <v>52</v>
       </c>
-      <c r="C37" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" t="s">
-        <v>54</v>
-      </c>
       <c r="E37" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" t="s">
         <v>55</v>
       </c>
-      <c r="C38" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" t="s">
-        <v>57</v>
-      </c>
       <c r="E38" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" t="s">
         <v>59</v>
-      </c>
-      <c r="C39" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" t="s">
         <v>62</v>
       </c>
-      <c r="C40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" t="s">
-        <v>64</v>
-      </c>
       <c r="E40" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" t="s">
         <v>65</v>
       </c>
-      <c r="C41" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" t="s">
-        <v>67</v>
-      </c>
       <c r="E41" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" t="s">
         <v>69</v>
-      </c>
-      <c r="C42" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" t="s">
-        <v>71</v>
-      </c>
-      <c r="E42" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" t="s">
         <v>73</v>
-      </c>
-      <c r="C43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" t="s">
-        <v>75</v>
-      </c>
-      <c r="E43" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" t="s">
         <v>77</v>
-      </c>
-      <c r="C44" t="s">
-        <v>78</v>
-      </c>
-      <c r="D44" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" t="s">
         <v>81</v>
-      </c>
-      <c r="C45" t="s">
-        <v>82</v>
-      </c>
-      <c r="D45" t="s">
-        <v>83</v>
-      </c>
-      <c r="E45" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" t="s">
+        <v>84</v>
+      </c>
+      <c r="E46" t="s">
         <v>85</v>
-      </c>
-      <c r="C46" t="s">
-        <v>86</v>
-      </c>
-      <c r="D46" t="s">
-        <v>44</v>
-      </c>
-      <c r="E46" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47" t="s">
         <v>88</v>
-      </c>
-      <c r="C47" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" t="s">
         <v>91</v>
       </c>
-      <c r="C48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" t="s">
-        <v>93</v>
-      </c>
       <c r="E48" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="B49" t="s">
+        <v>92</v>
+      </c>
+      <c r="C49" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" t="s">
         <v>95</v>
-      </c>
-      <c r="C49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D49" t="s">
-        <v>97</v>
-      </c>
-      <c r="E49" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="B50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" t="s">
         <v>98</v>
       </c>
-      <c r="C50" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" t="s">
-        <v>71</v>
-      </c>
       <c r="E50" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="B51" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" t="s">
         <v>100</v>
       </c>
-      <c r="C51" t="s">
-        <v>101</v>
-      </c>
       <c r="D51" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="E51" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="B52" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" t="s">
         <v>104</v>
       </c>
-      <c r="C52" t="s">
+    </row>
+    <row r="53" spans="1:5">
+      <c r="B53" t="s">
         <v>105</v>
       </c>
-      <c r="D52" t="s">
+      <c r="C53" t="s">
         <v>106</v>
       </c>
-      <c r="E52" t="s">
+      <c r="D53" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="1" t="s">
+      <c r="E53" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
-      <c r="B56" t="s">
+    <row r="55" spans="1:5">
+      <c r="A55" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="C56" t="s">
-        <v>110</v>
-      </c>
-      <c r="D56" t="s">
-        <v>111</v>
-      </c>
-      <c r="E56" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="B57" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" t="s">
+        <v>112</v>
+      </c>
+      <c r="E57" t="s">
         <v>113</v>
-      </c>
-      <c r="C57" t="s">
-        <v>114</v>
-      </c>
-      <c r="D57" t="s">
-        <v>115</v>
-      </c>
-      <c r="E57" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="B58" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D58" t="s">
-        <v>28</v>
+        <v>116</v>
       </c>
       <c r="E58" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="B59" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
       <c r="D59" t="s">
-        <v>118</v>
+        <v>29</v>
       </c>
       <c r="E59" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="B60" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60" t="s">
         <v>119</v>
       </c>
-      <c r="C60" t="s">
-        <v>120</v>
-      </c>
-      <c r="D60" t="s">
-        <v>121</v>
-      </c>
       <c r="E60" t="s">
-        <v>122</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="B61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61" t="s">
+        <v>122</v>
+      </c>
+      <c r="E61" t="s">
         <v>123</v>
-      </c>
-      <c r="C61" t="s">
-        <v>124</v>
-      </c>
-      <c r="D61" t="s">
-        <v>125</v>
-      </c>
-      <c r="E61" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="B62" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" t="s">
+        <v>125</v>
+      </c>
+      <c r="D62" t="s">
+        <v>126</v>
+      </c>
+      <c r="E62" t="s">
         <v>127</v>
-      </c>
-      <c r="C62" t="s">
-        <v>128</v>
-      </c>
-      <c r="D62" t="s">
-        <v>125</v>
-      </c>
-      <c r="E62" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="B63" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" t="s">
         <v>129</v>
       </c>
-      <c r="C63" t="s">
-        <v>130</v>
-      </c>
       <c r="D63" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E63" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="B64" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" t="s">
+        <v>131</v>
+      </c>
+      <c r="D64" t="s">
         <v>132</v>
       </c>
-      <c r="C64" t="s">
-        <v>133</v>
-      </c>
-      <c r="D64" t="s">
-        <v>134</v>
-      </c>
       <c r="E64" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="2:5">
       <c r="B65" t="s">
+        <v>133</v>
+      </c>
+      <c r="C65" t="s">
+        <v>134</v>
+      </c>
+      <c r="D65" t="s">
+        <v>135</v>
+      </c>
+      <c r="E65" t="s">
         <v>136</v>
-      </c>
-      <c r="C65" t="s">
-        <v>137</v>
-      </c>
-      <c r="D65" t="s">
-        <v>138</v>
-      </c>
-      <c r="E65" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="66" spans="2:5">
       <c r="B66" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" t="s">
+        <v>139</v>
+      </c>
+      <c r="E66" t="s">
         <v>140</v>
-      </c>
-      <c r="C66" t="s">
-        <v>141</v>
-      </c>
-      <c r="D66" t="s">
-        <v>142</v>
-      </c>
-      <c r="E66" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="67" spans="2:5">
       <c r="B67" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67" t="s">
+        <v>142</v>
+      </c>
+      <c r="D67" t="s">
         <v>143</v>
       </c>
-      <c r="C67" t="s">
-        <v>144</v>
-      </c>
-      <c r="D67" t="s">
-        <v>145</v>
-      </c>
       <c r="E67" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="2:5">
       <c r="B68" t="s">
+        <v>144</v>
+      </c>
+      <c r="C68" t="s">
+        <v>145</v>
+      </c>
+      <c r="D68" t="s">
         <v>146</v>
       </c>
-      <c r="C68" t="s">
-        <v>147</v>
-      </c>
-      <c r="D68" t="s">
-        <v>148</v>
-      </c>
       <c r="E68" t="s">
-        <v>149</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="2:5">
       <c r="B69" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69" t="s">
+        <v>149</v>
+      </c>
+      <c r="E69" t="s">
         <v>150</v>
-      </c>
-      <c r="C69" t="s">
-        <v>151</v>
-      </c>
-      <c r="D69" t="s">
-        <v>152</v>
-      </c>
-      <c r="E69" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="70" spans="2:5">
       <c r="B70" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C70" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D70" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E70" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="2:5">
       <c r="B71" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" t="s">
+        <v>152</v>
+      </c>
+      <c r="D71" t="s">
+        <v>153</v>
+      </c>
+      <c r="E71" t="s">
         <v>154</v>
-      </c>
-      <c r="C71" t="s">
-        <v>155</v>
-      </c>
-      <c r="D71" t="s">
-        <v>156</v>
-      </c>
-      <c r="E71" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="72" spans="2:5">
       <c r="B72" t="s">
+        <v>155</v>
+      </c>
+      <c r="C72" t="s">
+        <v>156</v>
+      </c>
+      <c r="D72" t="s">
         <v>157</v>
       </c>
-      <c r="C72" t="s">
-        <v>158</v>
-      </c>
-      <c r="D72" t="s">
-        <v>159</v>
-      </c>
       <c r="E72" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="2:5">
       <c r="B73" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" t="s">
+        <v>159</v>
+      </c>
+      <c r="D73" t="s">
         <v>160</v>
       </c>
-      <c r="C73" t="s">
-        <v>161</v>
-      </c>
-      <c r="D73" t="s">
-        <v>162</v>
-      </c>
       <c r="E73" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="2:5">
       <c r="B74" t="s">
+        <v>161</v>
+      </c>
+      <c r="C74" t="s">
+        <v>162</v>
+      </c>
+      <c r="D74" t="s">
         <v>163</v>
       </c>
-      <c r="C74" t="s">
-        <v>164</v>
-      </c>
-      <c r="D74" t="s">
-        <v>165</v>
-      </c>
       <c r="E74" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="2:5">
       <c r="B75" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75" t="s">
+        <v>165</v>
+      </c>
+      <c r="D75" t="s">
         <v>166</v>
       </c>
-      <c r="C75" t="s">
-        <v>167</v>
-      </c>
-      <c r="D75" t="s">
-        <v>168</v>
-      </c>
       <c r="E75" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="2:5">
       <c r="B76" t="s">
+        <v>167</v>
+      </c>
+      <c r="C76" t="s">
+        <v>168</v>
+      </c>
+      <c r="D76" t="s">
         <v>169</v>
       </c>
-      <c r="C76" t="s">
-        <v>170</v>
-      </c>
-      <c r="D76" t="s">
-        <v>171</v>
-      </c>
       <c r="E76" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="2:5">
       <c r="B77" t="s">
+        <v>170</v>
+      </c>
+      <c r="C77" t="s">
+        <v>171</v>
+      </c>
+      <c r="D77" t="s">
         <v>172</v>
       </c>
-      <c r="C77" t="s">
-        <v>173</v>
-      </c>
-      <c r="D77" t="s">
-        <v>174</v>
-      </c>
       <c r="E77" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="2:5">
       <c r="B78" t="s">
+        <v>173</v>
+      </c>
+      <c r="C78" t="s">
+        <v>174</v>
+      </c>
+      <c r="D78" t="s">
         <v>175</v>
       </c>
-      <c r="C78" t="s">
-        <v>176</v>
-      </c>
-      <c r="D78" t="s">
-        <v>177</v>
-      </c>
       <c r="E78" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="2:5">
       <c r="B79" t="s">
+        <v>176</v>
+      </c>
+      <c r="C79" t="s">
+        <v>177</v>
+      </c>
+      <c r="D79" t="s">
         <v>178</v>
       </c>
-      <c r="C79" t="s">
+      <c r="E79" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5">
+      <c r="B80" t="s">
         <v>179</v>
       </c>
-      <c r="D79" t="s">
+      <c r="C80" t="s">
         <v>180</v>
       </c>
-      <c r="E79" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="1" t="s">
+      <c r="D80" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="B83" t="s">
+      <c r="E80" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C83" t="s">
-        <v>183</v>
-      </c>
-      <c r="D83" t="s">
-        <v>184</v>
-      </c>
-      <c r="E83" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="B84" t="s">
+        <v>183</v>
+      </c>
+      <c r="C84" t="s">
+        <v>184</v>
+      </c>
+      <c r="D84" t="s">
         <v>185</v>
       </c>
-      <c r="C84" t="s">
+      <c r="E84" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D84" t="s">
-        <v>187</v>
-      </c>
-      <c r="E84" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="B85" t="s">
-        <v>188</v>
-      </c>
-      <c r="C85" t="s">
-        <v>189</v>
-      </c>
-      <c r="D85" t="s">
-        <v>190</v>
-      </c>
-      <c r="E85" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="B86" t="s">
-        <v>192</v>
-      </c>
-      <c r="C86" t="s">
-        <v>193</v>
-      </c>
-      <c r="D86" t="s">
-        <v>194</v>
-      </c>
-      <c r="E86" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="B87" t="s">
-        <v>196</v>
-      </c>
-      <c r="C87" t="s">
-        <v>197</v>
-      </c>
-      <c r="D87" t="s">
-        <v>198</v>
-      </c>
-      <c r="E87" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="B88" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="C88" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="D88" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="E88" t="s">
-        <v>203</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="B89" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="C89" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="D89" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="E89" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="B90" t="s">
+        <v>193</v>
+      </c>
+      <c r="C90" t="s">
+        <v>194</v>
+      </c>
+      <c r="D90" t="s">
+        <v>195</v>
+      </c>
+      <c r="E90" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="B91" t="s">
+        <v>197</v>
+      </c>
+      <c r="C91" t="s">
+        <v>198</v>
+      </c>
+      <c r="D91" t="s">
+        <v>199</v>
+      </c>
+      <c r="E91" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="B92" t="s">
+        <v>201</v>
+      </c>
+      <c r="C92" t="s">
+        <v>202</v>
+      </c>
+      <c r="D92" t="s">
+        <v>203</v>
+      </c>
+      <c r="E92" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="B93" t="s">
+        <v>205</v>
+      </c>
+      <c r="C93" t="s">
+        <v>206</v>
+      </c>
+      <c r="D93" t="s">
         <v>207</v>
       </c>
-      <c r="C90" t="s">
+      <c r="E93" t="s">
         <v>208</v>
-      </c>
-      <c r="D90" t="s">
-        <v>209</v>
-      </c>
-      <c r="E90" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="B94" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="C94" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="D94" t="s">
-        <v>184</v>
+        <v>211</v>
       </c>
       <c r="E94" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="B95" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="C95" t="s">
-        <v>186</v>
+        <v>213</v>
       </c>
       <c r="D95" t="s">
-        <v>187</v>
+        <v>214</v>
       </c>
       <c r="E95" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
-      <c r="B96" t="s">
-        <v>188</v>
-      </c>
-      <c r="C96" t="s">
-        <v>189</v>
-      </c>
-      <c r="D96" t="s">
-        <v>190</v>
-      </c>
-      <c r="E96" t="s">
-        <v>191</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97" spans="1:5">
-      <c r="B97" t="s">
-        <v>192</v>
-      </c>
-      <c r="C97" t="s">
-        <v>193</v>
-      </c>
-      <c r="D97" t="s">
-        <v>194</v>
-      </c>
-      <c r="E97" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="B98" t="s">
-        <v>211</v>
-      </c>
-      <c r="C98" t="s">
-        <v>212</v>
-      </c>
-      <c r="D98" t="s">
-        <v>213</v>
-      </c>
-      <c r="E98" t="s">
-        <v>191</v>
+      <c r="A97" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="B99" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C99" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D99" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E99" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="B100" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C100" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D100" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="E100" t="s">
-        <v>203</v>
+        <v>77</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="B101" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C101" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="D101" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="E101" t="s">
-        <v>34</v>
+        <v>196</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="B102" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C102" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D102" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E102" t="s">
-        <v>34</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="B103" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C103" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D103" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E103" t="s">
-        <v>34</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="B104" t="s">
+        <v>201</v>
+      </c>
+      <c r="C104" t="s">
+        <v>202</v>
+      </c>
+      <c r="D104" t="s">
+        <v>203</v>
+      </c>
+      <c r="E104" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="1" t="s">
-        <v>217</v>
+      <c r="B105" t="s">
+        <v>205</v>
+      </c>
+      <c r="C105" t="s">
+        <v>206</v>
+      </c>
+      <c r="D105" t="s">
+        <v>207</v>
+      </c>
+      <c r="E105" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="B106" t="s">
+        <v>209</v>
+      </c>
+      <c r="C106" t="s">
+        <v>210</v>
+      </c>
+      <c r="D106" t="s">
+        <v>211</v>
+      </c>
+      <c r="E106" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="B107" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C107" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D107" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E107" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="B108" t="s">
+        <v>219</v>
+      </c>
+      <c r="C108" t="s">
+        <v>220</v>
+      </c>
+      <c r="D108" t="s">
         <v>221</v>
       </c>
-      <c r="C108" t="s">
+      <c r="E108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="D108" t="s">
-        <v>223</v>
-      </c>
-      <c r="E108" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
-      <c r="B109" t="s">
-        <v>224</v>
-      </c>
-      <c r="C109" t="s">
-        <v>225</v>
-      </c>
-      <c r="D109" t="s">
-        <v>226</v>
-      </c>
-      <c r="E109" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
-      <c r="B110" t="s">
-        <v>227</v>
-      </c>
-      <c r="C110" t="s">
-        <v>228</v>
-      </c>
-      <c r="D110" t="s">
-        <v>229</v>
-      </c>
-      <c r="E110" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
-      <c r="B111" t="s">
-        <v>230</v>
-      </c>
-      <c r="C111" t="s">
-        <v>231</v>
-      </c>
-      <c r="D111" t="s">
-        <v>232</v>
-      </c>
-      <c r="E111" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="B112" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C112" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="D112" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="E112" t="s">
-        <v>236</v>
+        <v>35</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="B113" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="C113" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D113" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="E113" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="B114" t="s">
+        <v>229</v>
+      </c>
+      <c r="C114" t="s">
+        <v>230</v>
+      </c>
+      <c r="D114" t="s">
+        <v>231</v>
+      </c>
+      <c r="E114" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="B115" t="s">
+        <v>232</v>
+      </c>
+      <c r="C115" t="s">
+        <v>233</v>
+      </c>
+      <c r="D115" t="s">
+        <v>234</v>
+      </c>
+      <c r="E115" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="B116" t="s">
+        <v>235</v>
+      </c>
+      <c r="C116" t="s">
+        <v>236</v>
+      </c>
+      <c r="D116" t="s">
+        <v>237</v>
+      </c>
+      <c r="E116" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="B117" t="s">
+        <v>238</v>
+      </c>
+      <c r="C117" t="s">
+        <v>239</v>
+      </c>
+      <c r="D117" t="s">
         <v>240</v>
       </c>
-      <c r="C114" t="s">
+      <c r="E117" t="s">
         <v>241</v>
-      </c>
-      <c r="D114" t="s">
-        <v>242</v>
-      </c>
-      <c r="E114" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
-      <c r="A116" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="B118" t="s">
+        <v>242</v>
+      </c>
+      <c r="C118" t="s">
+        <v>243</v>
+      </c>
+      <c r="D118" t="s">
         <v>244</v>
       </c>
-      <c r="C118" t="s">
-        <v>245</v>
-      </c>
-      <c r="D118" t="s">
-        <v>246</v>
-      </c>
       <c r="E118" t="s">
-        <v>247</v>
+        <v>35</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="B119" t="s">
+        <v>245</v>
+      </c>
+      <c r="C119" t="s">
+        <v>246</v>
+      </c>
+      <c r="D119" t="s">
+        <v>247</v>
+      </c>
+      <c r="E119" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C119" t="s">
-        <v>245</v>
-      </c>
-      <c r="D119" t="s">
-        <v>246</v>
-      </c>
-      <c r="E119" t="s">
+    </row>
+    <row r="123" spans="1:5">
+      <c r="B123" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
-      <c r="B120" t="s">
+      <c r="C123" t="s">
         <v>250</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D123" t="s">
         <v>251</v>
       </c>
-      <c r="D120" t="s">
+      <c r="E123" t="s">
         <v>252</v>
-      </c>
-      <c r="E120" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5">
-      <c r="A122" s="1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="B124" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="C124" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="D124" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="E124" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="B125" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="C125" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="D125" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="E125" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="B129" t="s">
+        <v>249</v>
+      </c>
+      <c r="C129" t="s">
+        <v>250</v>
+      </c>
+      <c r="D129" t="s">
+        <v>251</v>
+      </c>
+      <c r="E129" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="B130" t="s">
+        <v>253</v>
+      </c>
+      <c r="C130" t="s">
+        <v>250</v>
+      </c>
+      <c r="D130" t="s">
+        <v>251</v>
+      </c>
+      <c r="E130" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="129" spans="2:5">
-      <c r="B129" t="s">
-        <v>255</v>
-      </c>
-      <c r="C129" t="s">
-        <v>256</v>
-      </c>
-      <c r="D129" t="s">
-        <v>257</v>
-      </c>
-      <c r="E129" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5">
-      <c r="B130" t="s">
-        <v>258</v>
-      </c>
-      <c r="C130" t="s">
-        <v>256</v>
-      </c>
-      <c r="D130" t="s">
-        <v>257</v>
-      </c>
-      <c r="E130" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="131" spans="2:5">
-      <c r="B131" t="s">
+    <row r="132" spans="1:5">
+      <c r="A132" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C131" t="s">
+    </row>
+    <row r="134" spans="1:5">
+      <c r="B134" t="s">
         <v>260</v>
       </c>
-      <c r="D131" t="s">
+      <c r="C134" t="s">
         <v>261</v>
       </c>
-      <c r="E131" t="s">
+      <c r="D134" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="132" spans="2:5">
-      <c r="B132" t="s">
-        <v>259</v>
-      </c>
-      <c r="C132" t="s">
-        <v>260</v>
-      </c>
-      <c r="D132" t="s">
+      <c r="E134" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="B135" t="s">
+        <v>263</v>
+      </c>
+      <c r="C135" t="s">
         <v>261</v>
       </c>
-      <c r="E132" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="133" spans="2:5">
-      <c r="B133" t="s">
-        <v>263</v>
-      </c>
-      <c r="C133" t="s">
+      <c r="D135" t="s">
+        <v>262</v>
+      </c>
+      <c r="E135" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="B136" t="s">
         <v>264</v>
       </c>
-      <c r="D133" t="s">
-        <v>246</v>
-      </c>
-      <c r="E133" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5">
-      <c r="B134" t="s">
+      <c r="C136" t="s">
         <v>265</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D136" t="s">
+        <v>266</v>
+      </c>
+      <c r="E136" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="B137" t="s">
         <v>264</v>
       </c>
-      <c r="D134" t="s">
-        <v>246</v>
-      </c>
-      <c r="E134" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5">
-      <c r="B135" t="s">
-        <v>26</v>
-      </c>
-      <c r="C135" t="s">
-        <v>27</v>
-      </c>
-      <c r="D135" t="s">
-        <v>28</v>
-      </c>
-      <c r="E135" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5">
-      <c r="B136" t="s">
-        <v>26</v>
-      </c>
-      <c r="C136" t="s">
-        <v>27</v>
-      </c>
-      <c r="D136" t="s">
-        <v>28</v>
-      </c>
-      <c r="E136" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5">
-      <c r="B137" t="s">
+      <c r="C137" t="s">
+        <v>265</v>
+      </c>
+      <c r="D137" t="s">
         <v>266</v>
       </c>
-      <c r="C137" t="s">
+      <c r="E137" t="s">
         <v>267</v>
       </c>
-      <c r="D137" t="s">
+    </row>
+    <row r="138" spans="1:5">
+      <c r="B138" t="s">
         <v>268</v>
       </c>
-      <c r="E137" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="138" spans="2:5">
-      <c r="B138" t="s">
+      <c r="C138" t="s">
         <v>269</v>
       </c>
-      <c r="C138" t="s">
-        <v>267</v>
-      </c>
       <c r="D138" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="E138" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="B139" t="s">
         <v>270</v>
       </c>
       <c r="C139" t="s">
+        <v>269</v>
+      </c>
+      <c r="D139" t="s">
+        <v>251</v>
+      </c>
+      <c r="E139" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="B140" t="s">
+        <v>27</v>
+      </c>
+      <c r="C140" t="s">
+        <v>28</v>
+      </c>
+      <c r="D140" t="s">
+        <v>29</v>
+      </c>
+      <c r="E140" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="B141" t="s">
+        <v>27</v>
+      </c>
+      <c r="C141" t="s">
+        <v>28</v>
+      </c>
+      <c r="D141" t="s">
+        <v>29</v>
+      </c>
+      <c r="E141" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="B142" t="s">
         <v>271</v>
       </c>
-      <c r="D139" t="s">
+      <c r="C142" t="s">
         <v>272</v>
       </c>
-      <c r="E139" t="s">
+      <c r="D142" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="140" spans="2:5">
-      <c r="B140" t="s">
+      <c r="E142" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="B143" t="s">
+        <v>274</v>
+      </c>
+      <c r="C143" t="s">
+        <v>272</v>
+      </c>
+      <c r="D143" t="s">
+        <v>273</v>
+      </c>
+      <c r="E143" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="B144" t="s">
+        <v>275</v>
+      </c>
+      <c r="C144" t="s">
+        <v>276</v>
+      </c>
+      <c r="D144" t="s">
+        <v>277</v>
+      </c>
+      <c r="E144" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5">
+      <c r="B145" t="s">
+        <v>275</v>
+      </c>
+      <c r="C145" t="s">
+        <v>276</v>
+      </c>
+      <c r="D145" t="s">
+        <v>277</v>
+      </c>
+      <c r="E145" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5">
+      <c r="B146" t="s">
+        <v>280</v>
+      </c>
+      <c r="C146" t="s">
+        <v>281</v>
+      </c>
+      <c r="D146" t="s">
+        <v>221</v>
+      </c>
+      <c r="E146" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5">
+      <c r="B147" t="s">
+        <v>283</v>
+      </c>
+      <c r="C147" t="s">
+        <v>281</v>
+      </c>
+      <c r="D147" t="s">
+        <v>221</v>
+      </c>
+      <c r="E147" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5">
+      <c r="B148" t="s">
+        <v>201</v>
+      </c>
+      <c r="C148" t="s">
+        <v>202</v>
+      </c>
+      <c r="D148" t="s">
+        <v>203</v>
+      </c>
+      <c r="E148" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5">
+      <c r="B149" t="s">
+        <v>284</v>
+      </c>
+      <c r="C149" t="s">
+        <v>202</v>
+      </c>
+      <c r="D149" t="s">
+        <v>203</v>
+      </c>
+      <c r="E149" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5">
+      <c r="B150" t="s">
+        <v>151</v>
+      </c>
+      <c r="C150" t="s">
+        <v>152</v>
+      </c>
+      <c r="D150" t="s">
+        <v>153</v>
+      </c>
+      <c r="E150" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5">
+      <c r="B151" t="s">
+        <v>151</v>
+      </c>
+      <c r="C151" t="s">
+        <v>152</v>
+      </c>
+      <c r="D151" t="s">
+        <v>153</v>
+      </c>
+      <c r="E151" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5">
+      <c r="B152" t="s">
+        <v>286</v>
+      </c>
+      <c r="C152" t="s">
+        <v>287</v>
+      </c>
+      <c r="D152" t="s">
+        <v>288</v>
+      </c>
+      <c r="E152" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5">
+      <c r="B153" t="s">
+        <v>289</v>
+      </c>
+      <c r="C153" t="s">
+        <v>287</v>
+      </c>
+      <c r="D153" t="s">
+        <v>288</v>
+      </c>
+      <c r="E153" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5">
+      <c r="B154" t="s">
+        <v>291</v>
+      </c>
+      <c r="C154" t="s">
+        <v>292</v>
+      </c>
+      <c r="D154" t="s">
+        <v>293</v>
+      </c>
+      <c r="E154" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5">
+      <c r="B155" t="s">
+        <v>294</v>
+      </c>
+      <c r="C155" t="s">
+        <v>292</v>
+      </c>
+      <c r="D155" t="s">
+        <v>293</v>
+      </c>
+      <c r="E155" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5">
+      <c r="B156" t="s">
+        <v>249</v>
+      </c>
+      <c r="C156" t="s">
+        <v>250</v>
+      </c>
+      <c r="D156" t="s">
+        <v>251</v>
+      </c>
+      <c r="E156" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5">
+      <c r="B157" t="s">
+        <v>253</v>
+      </c>
+      <c r="C157" t="s">
+        <v>250</v>
+      </c>
+      <c r="D157" t="s">
+        <v>251</v>
+      </c>
+      <c r="E157" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="158" spans="2:5">
+      <c r="B158" t="s">
+        <v>295</v>
+      </c>
+      <c r="C158" t="s">
+        <v>296</v>
+      </c>
+      <c r="D158" t="s">
+        <v>297</v>
+      </c>
+      <c r="E158" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5">
+      <c r="B159" t="s">
+        <v>295</v>
+      </c>
+      <c r="C159" t="s">
+        <v>296</v>
+      </c>
+      <c r="D159" t="s">
+        <v>297</v>
+      </c>
+      <c r="E159" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="B163" t="s">
+        <v>36</v>
+      </c>
+      <c r="C163" t="s">
+        <v>33</v>
+      </c>
+      <c r="D163" t="s">
+        <v>34</v>
+      </c>
+      <c r="E163" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="B164" t="s">
+        <v>260</v>
+      </c>
+      <c r="C164" t="s">
+        <v>261</v>
+      </c>
+      <c r="D164" t="s">
+        <v>262</v>
+      </c>
+      <c r="E164" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="B165" t="s">
+        <v>263</v>
+      </c>
+      <c r="C165" t="s">
+        <v>261</v>
+      </c>
+      <c r="D165" t="s">
+        <v>262</v>
+      </c>
+      <c r="E165" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="B166" t="s">
         <v>270</v>
       </c>
-      <c r="C140" t="s">
-        <v>271</v>
-      </c>
-      <c r="D140" t="s">
+      <c r="C166" t="s">
+        <v>269</v>
+      </c>
+      <c r="D166" t="s">
+        <v>251</v>
+      </c>
+      <c r="E166" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="B167" t="s">
+        <v>50</v>
+      </c>
+      <c r="C167" t="s">
+        <v>51</v>
+      </c>
+      <c r="D167" t="s">
+        <v>52</v>
+      </c>
+      <c r="E167" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="B168" t="s">
+        <v>274</v>
+      </c>
+      <c r="C168" t="s">
         <v>272</v>
       </c>
-      <c r="E140" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="141" spans="2:5">
-      <c r="B141" t="s">
-        <v>275</v>
-      </c>
-      <c r="C141" t="s">
-        <v>276</v>
-      </c>
-      <c r="D141" t="s">
-        <v>216</v>
-      </c>
-      <c r="E141" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="142" spans="2:5">
-      <c r="B142" t="s">
-        <v>278</v>
-      </c>
-      <c r="C142" t="s">
-        <v>276</v>
-      </c>
-      <c r="D142" t="s">
-        <v>216</v>
-      </c>
-      <c r="E142" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="143" spans="2:5">
-      <c r="B143" t="s">
-        <v>196</v>
-      </c>
-      <c r="C143" t="s">
-        <v>197</v>
-      </c>
-      <c r="D143" t="s">
-        <v>198</v>
-      </c>
-      <c r="E143" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="144" spans="2:5">
-      <c r="B144" t="s">
-        <v>279</v>
-      </c>
-      <c r="C144" t="s">
-        <v>197</v>
-      </c>
-      <c r="D144" t="s">
-        <v>198</v>
-      </c>
-      <c r="E144" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5">
-      <c r="B145" t="s">
+      <c r="D168" t="s">
+        <v>273</v>
+      </c>
+      <c r="E168" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="B169" t="s">
+        <v>299</v>
+      </c>
+      <c r="C169" t="s">
+        <v>300</v>
+      </c>
+      <c r="D169" t="s">
+        <v>301</v>
+      </c>
+      <c r="E169" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="B170" t="s">
+        <v>232</v>
+      </c>
+      <c r="C170" t="s">
+        <v>233</v>
+      </c>
+      <c r="D170" t="s">
+        <v>234</v>
+      </c>
+      <c r="E170" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="B171" t="s">
+        <v>302</v>
+      </c>
+      <c r="C171" t="s">
+        <v>303</v>
+      </c>
+      <c r="D171" t="s">
+        <v>304</v>
+      </c>
+      <c r="E171" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="B172" t="s">
+        <v>283</v>
+      </c>
+      <c r="C172" t="s">
+        <v>281</v>
+      </c>
+      <c r="D172" t="s">
+        <v>221</v>
+      </c>
+      <c r="E172" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="B173" t="s">
+        <v>284</v>
+      </c>
+      <c r="C173" t="s">
+        <v>202</v>
+      </c>
+      <c r="D173" t="s">
+        <v>203</v>
+      </c>
+      <c r="E173" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="B174" t="s">
+        <v>289</v>
+      </c>
+      <c r="C174" t="s">
+        <v>287</v>
+      </c>
+      <c r="D174" t="s">
+        <v>288</v>
+      </c>
+      <c r="E174" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="B175" t="s">
+        <v>294</v>
+      </c>
+      <c r="C175" t="s">
+        <v>292</v>
+      </c>
+      <c r="D175" t="s">
+        <v>293</v>
+      </c>
+      <c r="E175" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="B176" t="s">
+        <v>306</v>
+      </c>
+      <c r="C176" t="s">
+        <v>307</v>
+      </c>
+      <c r="D176" t="s">
+        <v>189</v>
+      </c>
+      <c r="E176" t="s">
         <v>150</v>
       </c>
-      <c r="C145" t="s">
-        <v>151</v>
-      </c>
-      <c r="D145" t="s">
-        <v>152</v>
-      </c>
-      <c r="E145" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5">
-      <c r="B146" t="s">
-        <v>150</v>
-      </c>
-      <c r="C146" t="s">
-        <v>151</v>
-      </c>
-      <c r="D146" t="s">
-        <v>152</v>
-      </c>
-      <c r="E146" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5">
-      <c r="B147" t="s">
-        <v>281</v>
-      </c>
-      <c r="C147" t="s">
-        <v>282</v>
-      </c>
-      <c r="D147" t="s">
-        <v>283</v>
-      </c>
-      <c r="E147" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5">
-      <c r="B148" t="s">
-        <v>284</v>
-      </c>
-      <c r="C148" t="s">
-        <v>282</v>
-      </c>
-      <c r="D148" t="s">
-        <v>283</v>
-      </c>
-      <c r="E148" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5">
-      <c r="B149" t="s">
-        <v>286</v>
-      </c>
-      <c r="C149" t="s">
-        <v>287</v>
-      </c>
-      <c r="D149" t="s">
-        <v>288</v>
-      </c>
-      <c r="E149" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5">
-      <c r="B150" t="s">
-        <v>289</v>
-      </c>
-      <c r="C150" t="s">
-        <v>287</v>
-      </c>
-      <c r="D150" t="s">
-        <v>288</v>
-      </c>
-      <c r="E150" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5">
-      <c r="B151" t="s">
-        <v>244</v>
-      </c>
-      <c r="C151" t="s">
-        <v>245</v>
-      </c>
-      <c r="D151" t="s">
-        <v>246</v>
-      </c>
-      <c r="E151" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5">
-      <c r="B152" t="s">
-        <v>248</v>
-      </c>
-      <c r="C152" t="s">
-        <v>245</v>
-      </c>
-      <c r="D152" t="s">
-        <v>246</v>
-      </c>
-      <c r="E152" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5">
-      <c r="B153" t="s">
-        <v>290</v>
-      </c>
-      <c r="C153" t="s">
-        <v>291</v>
-      </c>
-      <c r="D153" t="s">
-        <v>292</v>
-      </c>
-      <c r="E153" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5">
-      <c r="B154" t="s">
-        <v>290</v>
-      </c>
-      <c r="C154" t="s">
-        <v>291</v>
-      </c>
-      <c r="D154" t="s">
-        <v>292</v>
-      </c>
-      <c r="E154" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5">
-      <c r="A156" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5">
-      <c r="B158" t="s">
-        <v>35</v>
-      </c>
-      <c r="C158" t="s">
-        <v>32</v>
-      </c>
-      <c r="D158" t="s">
-        <v>33</v>
-      </c>
-      <c r="E158" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5">
-      <c r="B159" t="s">
-        <v>255</v>
-      </c>
-      <c r="C159" t="s">
-        <v>256</v>
-      </c>
-      <c r="D159" t="s">
-        <v>257</v>
-      </c>
-      <c r="E159" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5">
-      <c r="B160" t="s">
-        <v>258</v>
-      </c>
-      <c r="C160" t="s">
-        <v>256</v>
-      </c>
-      <c r="D160" t="s">
-        <v>257</v>
-      </c>
-      <c r="E160" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="161" spans="2:5">
-      <c r="B161" t="s">
-        <v>265</v>
-      </c>
-      <c r="C161" t="s">
-        <v>264</v>
-      </c>
-      <c r="D161" t="s">
-        <v>246</v>
-      </c>
-      <c r="E161" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="162" spans="2:5">
-      <c r="B162" t="s">
-        <v>49</v>
-      </c>
-      <c r="C162" t="s">
-        <v>50</v>
-      </c>
-      <c r="D162" t="s">
-        <v>51</v>
-      </c>
-      <c r="E162" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="163" spans="2:5">
-      <c r="B163" t="s">
-        <v>269</v>
-      </c>
-      <c r="C163" t="s">
-        <v>267</v>
-      </c>
-      <c r="D163" t="s">
-        <v>268</v>
-      </c>
-      <c r="E163" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="164" spans="2:5">
-      <c r="B164" t="s">
-        <v>294</v>
-      </c>
-      <c r="C164" t="s">
-        <v>295</v>
-      </c>
-      <c r="D164" t="s">
-        <v>296</v>
-      </c>
-      <c r="E164" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="165" spans="2:5">
-      <c r="B165" t="s">
-        <v>227</v>
-      </c>
-      <c r="C165" t="s">
-        <v>228</v>
-      </c>
-      <c r="D165" t="s">
-        <v>229</v>
-      </c>
-      <c r="E165" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="166" spans="2:5">
-      <c r="B166" t="s">
-        <v>297</v>
-      </c>
-      <c r="C166" t="s">
-        <v>298</v>
-      </c>
-      <c r="D166" t="s">
-        <v>299</v>
-      </c>
-      <c r="E166" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="167" spans="2:5">
-      <c r="B167" t="s">
-        <v>278</v>
-      </c>
-      <c r="C167" t="s">
-        <v>276</v>
-      </c>
-      <c r="D167" t="s">
-        <v>216</v>
-      </c>
-      <c r="E167" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="168" spans="2:5">
-      <c r="B168" t="s">
-        <v>279</v>
-      </c>
-      <c r="C168" t="s">
-        <v>197</v>
-      </c>
-      <c r="D168" t="s">
-        <v>198</v>
-      </c>
-      <c r="E168" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="169" spans="2:5">
-      <c r="B169" t="s">
-        <v>284</v>
-      </c>
-      <c r="C169" t="s">
-        <v>282</v>
-      </c>
-      <c r="D169" t="s">
-        <v>283</v>
-      </c>
-      <c r="E169" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="170" spans="2:5">
-      <c r="B170" t="s">
-        <v>289</v>
-      </c>
-      <c r="C170" t="s">
-        <v>287</v>
-      </c>
-      <c r="D170" t="s">
-        <v>288</v>
-      </c>
-      <c r="E170" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="171" spans="2:5">
-      <c r="B171" t="s">
-        <v>301</v>
-      </c>
-      <c r="C171" t="s">
-        <v>302</v>
-      </c>
-      <c r="D171" t="s">
-        <v>184</v>
-      </c>
-      <c r="E171" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="172" spans="2:5">
-      <c r="B172" t="s">
-        <v>303</v>
-      </c>
-      <c r="C172" t="s">
-        <v>304</v>
-      </c>
-      <c r="D172" t="s">
-        <v>305</v>
-      </c>
-      <c r="E172" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="173" spans="2:5">
-      <c r="B173" t="s">
-        <v>248</v>
-      </c>
-      <c r="C173" t="s">
-        <v>245</v>
-      </c>
-      <c r="D173" t="s">
-        <v>246</v>
-      </c>
-      <c r="E173" t="s">
-        <v>249</v>
+    </row>
+    <row r="177" spans="2:5">
+      <c r="B177" t="s">
+        <v>308</v>
+      </c>
+      <c r="C177" t="s">
+        <v>309</v>
+      </c>
+      <c r="D177" t="s">
+        <v>310</v>
+      </c>
+      <c r="E177" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="178" spans="2:5">
+      <c r="B178" t="s">
+        <v>253</v>
+      </c>
+      <c r="C178" t="s">
+        <v>250</v>
+      </c>
+      <c r="D178" t="s">
+        <v>251</v>
+      </c>
+      <c r="E178" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>